<commit_message>
update dmn test case and update doc
</commit_message>
<xml_diff>
--- a/dmn.tool/docs/DMN-云田、古亭3台主变.xlsx
+++ b/dmn.tool/docs/DMN-云田、古亭3台主变.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="46">
   <si>
     <t>input</t>
   </si>
@@ -191,6 +191,10 @@
   </si>
   <si>
     <t>古亭主变下网的35%+云田主变下网之和越界</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -572,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -586,7 +590,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9:J9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -723,7 +727,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>9</v>

</xml_diff>